<commit_message>
updating and adding data translators and more testing
</commit_message>
<xml_diff>
--- a/data/published/2016_ColloffWadeStrange/testInput.xlsx
+++ b/data/published/2016_ColloffWadeStrange/testInput.xlsx
@@ -8,28 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lauramickes/Google Drive/Current/18Modelling Programming/pyWitness/data/published/2016_ColloffWadeStrange/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EC821C1-11A2-264E-91C2-D973C6154C8F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28071A07-B783-C840-A6C6-FF60973850D4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10640" yWindow="9520" windowWidth="33100" windowHeight="19140" xr2:uid="{9ED41D21-AD87-EA4A-9860-FFB390C24F36}"/>
+    <workbookView xWindow="10640" yWindow="8780" windowWidth="33100" windowHeight="19140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -39,21 +25,66 @@
     <t>Data translator</t>
   </si>
   <si>
+    <t>published_Colloff_2016()</t>
+  </si>
+  <si>
     <t>Model fit</t>
   </si>
   <si>
+    <t>IndependentObservation</t>
+  </si>
+  <si>
+    <t>Ensemble</t>
+  </si>
+  <si>
+    <t>Integration</t>
+  </si>
+  <si>
     <t>Parameter set</t>
   </si>
   <si>
+    <t>EqualVariance</t>
+  </si>
+  <si>
+    <t>UnequalVariance</t>
+  </si>
+  <si>
+    <t>Exclusions</t>
+  </si>
+  <si>
+    <t>{"exclude":"yes"}</t>
+  </si>
+  <si>
     <t>Condition</t>
   </si>
   <si>
-    <t>Exclusions</t>
+    <t>treatmentLabel replication</t>
+  </si>
+  <si>
+    <t>treatmentLabel nothing</t>
+  </si>
+  <si>
+    <t>treatmentLabel pixelation</t>
+  </si>
+  <si>
+    <t>treatmentLabel concealment</t>
   </si>
   <si>
     <t>Binning</t>
   </si>
   <si>
+    <t>[-1,60,80,100]</t>
+  </si>
+  <si>
+    <t>Parameter estimates</t>
+  </si>
+  <si>
+    <t>True</t>
+  </si>
+  <si>
+    <t>maxiter</t>
+  </si>
+  <si>
     <t>Model parameter</t>
   </si>
   <si>
@@ -108,6 +139,18 @@
     <t>c11</t>
   </si>
   <si>
+    <t>c12</t>
+  </si>
+  <si>
+    <t>c13</t>
+  </si>
+  <si>
+    <t>c14</t>
+  </si>
+  <si>
+    <t>c15</t>
+  </si>
+  <si>
     <t>niter</t>
   </si>
   <si>
@@ -117,36 +160,12 @@
     <t>chi-square</t>
   </si>
   <si>
-    <t>IndependentObservation</t>
-  </si>
-  <si>
-    <t>EqualVariance</t>
-  </si>
-  <si>
-    <t>maxiter</t>
-  </si>
-  <si>
-    <t>UnequalVariance</t>
-  </si>
-  <si>
-    <t>Ensemble</t>
-  </si>
-  <si>
-    <t>Integration</t>
-  </si>
-  <si>
-    <t>Parameter estimates</t>
-  </si>
-  <si>
-    <t>True</t>
+    <t>ndf</t>
   </si>
   <si>
     <t>chi2-per-ndf</t>
   </si>
   <si>
-    <t>ndf</t>
-  </si>
-  <si>
     <t>Descriptive stats</t>
   </si>
   <si>
@@ -159,18 +178,6 @@
     <t>number TP lineups</t>
   </si>
   <si>
-    <t>c12</t>
-  </si>
-  <si>
-    <t>c13</t>
-  </si>
-  <si>
-    <t>c14</t>
-  </si>
-  <si>
-    <t>c15</t>
-  </si>
-  <si>
     <t>correctID</t>
   </si>
   <si>
@@ -181,27 +188,6 @@
   </si>
   <si>
     <t>pAUC</t>
-  </si>
-  <si>
-    <t>[-1,60,80,100]</t>
-  </si>
-  <si>
-    <t>treatmentLabel replication</t>
-  </si>
-  <si>
-    <t>treatmentLabel nothing</t>
-  </si>
-  <si>
-    <t>treatmentLabel pixelation</t>
-  </si>
-  <si>
-    <t>treatmentLabel concealment</t>
-  </si>
-  <si>
-    <t>{"exclude":"yes"}</t>
-  </si>
-  <si>
-    <t>published_Colloff_2016()</t>
   </si>
 </sst>
 </file>
@@ -255,12 +241,12 @@
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -574,562 +560,563 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D299942-CAD7-8B42-80C6-6BA1FC3BDCD5}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Y43"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="117" zoomScaleNormal="117" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="18.83203125" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="25" width="35" style="2" bestFit="1" customWidth="1"/>
-    <col min="26" max="16384" width="10.83203125" style="2"/>
+    <col min="26" max="26" width="10.83203125" style="2" customWidth="1"/>
+    <col min="27" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>55</v>
+        <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>55</v>
+        <v>1</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>55</v>
+        <v>1</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>55</v>
+        <v>1</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>55</v>
+        <v>1</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>55</v>
+        <v>1</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>55</v>
+        <v>1</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>55</v>
+        <v>1</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>55</v>
+        <v>1</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>55</v>
+        <v>1</v>
       </c>
       <c r="L1" s="3" t="s">
-        <v>55</v>
+        <v>1</v>
       </c>
       <c r="M1" s="3" t="s">
-        <v>55</v>
+        <v>1</v>
       </c>
       <c r="N1" s="3" t="s">
-        <v>55</v>
+        <v>1</v>
       </c>
       <c r="O1" s="3" t="s">
-        <v>55</v>
+        <v>1</v>
       </c>
       <c r="P1" s="3" t="s">
-        <v>55</v>
+        <v>1</v>
       </c>
       <c r="Q1" s="3" t="s">
-        <v>55</v>
+        <v>1</v>
       </c>
       <c r="R1" s="3" t="s">
-        <v>55</v>
+        <v>1</v>
       </c>
       <c r="S1" s="3" t="s">
-        <v>55</v>
+        <v>1</v>
       </c>
       <c r="T1" s="3" t="s">
-        <v>55</v>
+        <v>1</v>
       </c>
       <c r="U1" s="3" t="s">
-        <v>55</v>
+        <v>1</v>
       </c>
       <c r="V1" s="3" t="s">
-        <v>55</v>
+        <v>1</v>
       </c>
       <c r="W1" s="3" t="s">
-        <v>55</v>
+        <v>1</v>
       </c>
       <c r="X1" s="3" t="s">
-        <v>55</v>
+        <v>1</v>
       </c>
       <c r="Y1" s="3" t="s">
-        <v>55</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
-        <v>1</v>
+      <c r="A2" t="s">
+        <v>2</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>27</v>
+        <v>3</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>27</v>
+        <v>3</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>31</v>
+        <v>4</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>31</v>
+        <v>4</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>32</v>
+        <v>5</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>32</v>
+        <v>5</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>27</v>
+        <v>3</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>27</v>
+        <v>3</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>31</v>
+        <v>4</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>31</v>
+        <v>4</v>
       </c>
       <c r="L2" s="4" t="s">
-        <v>32</v>
+        <v>5</v>
       </c>
       <c r="M2" s="4" t="s">
-        <v>32</v>
+        <v>5</v>
       </c>
       <c r="N2" s="4" t="s">
-        <v>27</v>
+        <v>3</v>
       </c>
       <c r="O2" s="4" t="s">
-        <v>27</v>
+        <v>3</v>
       </c>
       <c r="P2" s="4" t="s">
-        <v>31</v>
+        <v>4</v>
       </c>
       <c r="Q2" s="4" t="s">
-        <v>31</v>
+        <v>4</v>
       </c>
       <c r="R2" s="4" t="s">
-        <v>32</v>
+        <v>5</v>
       </c>
       <c r="S2" s="4" t="s">
-        <v>32</v>
+        <v>5</v>
       </c>
       <c r="T2" s="4" t="s">
-        <v>27</v>
+        <v>3</v>
       </c>
       <c r="U2" s="4" t="s">
-        <v>27</v>
+        <v>3</v>
       </c>
       <c r="V2" s="4" t="s">
-        <v>31</v>
+        <v>4</v>
       </c>
       <c r="W2" s="4" t="s">
-        <v>31</v>
+        <v>4</v>
       </c>
       <c r="X2" s="4" t="s">
-        <v>32</v>
+        <v>5</v>
       </c>
       <c r="Y2" s="4" t="s">
-        <v>32</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
-        <v>2</v>
+      <c r="A3" t="s">
+        <v>6</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>28</v>
+        <v>7</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>30</v>
+        <v>8</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>28</v>
+        <v>7</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>30</v>
+        <v>8</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>28</v>
+        <v>7</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>30</v>
+        <v>8</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>28</v>
+        <v>7</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>30</v>
+        <v>8</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>28</v>
+        <v>7</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>30</v>
+        <v>8</v>
       </c>
       <c r="L3" s="4" t="s">
-        <v>28</v>
+        <v>7</v>
       </c>
       <c r="M3" s="4" t="s">
-        <v>30</v>
+        <v>8</v>
       </c>
       <c r="N3" s="4" t="s">
-        <v>28</v>
+        <v>7</v>
       </c>
       <c r="O3" s="4" t="s">
-        <v>30</v>
+        <v>8</v>
       </c>
       <c r="P3" s="4" t="s">
-        <v>28</v>
+        <v>7</v>
       </c>
       <c r="Q3" s="4" t="s">
-        <v>30</v>
+        <v>8</v>
       </c>
       <c r="R3" s="4" t="s">
-        <v>28</v>
+        <v>7</v>
       </c>
       <c r="S3" s="4" t="s">
-        <v>30</v>
+        <v>8</v>
       </c>
       <c r="T3" s="4" t="s">
-        <v>28</v>
+        <v>7</v>
       </c>
       <c r="U3" s="4" t="s">
-        <v>30</v>
+        <v>8</v>
       </c>
       <c r="V3" s="4" t="s">
-        <v>28</v>
+        <v>7</v>
       </c>
       <c r="W3" s="4" t="s">
-        <v>30</v>
+        <v>8</v>
       </c>
       <c r="X3" s="4" t="s">
-        <v>28</v>
+        <v>7</v>
       </c>
       <c r="Y3" s="4" t="s">
-        <v>30</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
-        <v>4</v>
+      <c r="A4" t="s">
+        <v>9</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>54</v>
+        <v>10</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>54</v>
+        <v>10</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>54</v>
+        <v>10</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>54</v>
+        <v>10</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>54</v>
+        <v>10</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>54</v>
+        <v>10</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>54</v>
+        <v>10</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>54</v>
+        <v>10</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>54</v>
+        <v>10</v>
       </c>
       <c r="K4" s="4" t="s">
-        <v>54</v>
+        <v>10</v>
       </c>
       <c r="L4" s="4" t="s">
-        <v>54</v>
+        <v>10</v>
       </c>
       <c r="M4" s="4" t="s">
-        <v>54</v>
+        <v>10</v>
       </c>
       <c r="N4" s="4" t="s">
-        <v>54</v>
+        <v>10</v>
       </c>
       <c r="O4" s="4" t="s">
-        <v>54</v>
+        <v>10</v>
       </c>
       <c r="P4" s="4" t="s">
-        <v>54</v>
+        <v>10</v>
       </c>
       <c r="Q4" s="4" t="s">
-        <v>54</v>
+        <v>10</v>
       </c>
       <c r="R4" s="4" t="s">
-        <v>54</v>
+        <v>10</v>
       </c>
       <c r="S4" s="4" t="s">
-        <v>54</v>
+        <v>10</v>
       </c>
       <c r="T4" s="4" t="s">
-        <v>54</v>
+        <v>10</v>
       </c>
       <c r="U4" s="4" t="s">
-        <v>54</v>
+        <v>10</v>
       </c>
       <c r="V4" s="4" t="s">
-        <v>54</v>
+        <v>10</v>
       </c>
       <c r="W4" s="4" t="s">
-        <v>54</v>
+        <v>10</v>
       </c>
       <c r="X4" s="4" t="s">
-        <v>54</v>
+        <v>10</v>
       </c>
       <c r="Y4" s="4" t="s">
-        <v>54</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
-        <v>3</v>
+      <c r="A5" t="s">
+        <v>11</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>50</v>
+        <v>12</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>50</v>
+        <v>12</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>50</v>
+        <v>12</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>50</v>
+        <v>12</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>50</v>
+        <v>12</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>50</v>
+        <v>12</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>51</v>
+        <v>13</v>
       </c>
       <c r="I5" s="4" t="s">
-        <v>51</v>
+        <v>13</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>51</v>
+        <v>13</v>
       </c>
       <c r="K5" s="4" t="s">
-        <v>51</v>
+        <v>13</v>
       </c>
       <c r="L5" s="4" t="s">
-        <v>51</v>
+        <v>13</v>
       </c>
       <c r="M5" s="4" t="s">
-        <v>51</v>
+        <v>13</v>
       </c>
       <c r="N5" s="4" t="s">
-        <v>52</v>
+        <v>14</v>
       </c>
       <c r="O5" s="4" t="s">
-        <v>52</v>
+        <v>14</v>
       </c>
       <c r="P5" s="4" t="s">
-        <v>52</v>
+        <v>14</v>
       </c>
       <c r="Q5" s="4" t="s">
-        <v>52</v>
+        <v>14</v>
       </c>
       <c r="R5" s="4" t="s">
-        <v>52</v>
+        <v>14</v>
       </c>
       <c r="S5" s="4" t="s">
-        <v>52</v>
+        <v>14</v>
       </c>
       <c r="T5" s="4" t="s">
-        <v>53</v>
+        <v>15</v>
       </c>
       <c r="U5" s="4" t="s">
-        <v>53</v>
+        <v>15</v>
       </c>
       <c r="V5" s="4" t="s">
-        <v>53</v>
+        <v>15</v>
       </c>
       <c r="W5" s="4" t="s">
-        <v>53</v>
+        <v>15</v>
       </c>
       <c r="X5" s="4" t="s">
-        <v>53</v>
+        <v>15</v>
       </c>
       <c r="Y5" s="4" t="s">
-        <v>53</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
-        <v>5</v>
+      <c r="A6" t="s">
+        <v>16</v>
       </c>
       <c r="B6" t="s">
-        <v>49</v>
+        <v>17</v>
       </c>
       <c r="C6" t="s">
-        <v>49</v>
+        <v>17</v>
       </c>
       <c r="D6" t="s">
-        <v>49</v>
+        <v>17</v>
       </c>
       <c r="E6" t="s">
-        <v>49</v>
+        <v>17</v>
       </c>
       <c r="F6" t="s">
-        <v>49</v>
+        <v>17</v>
       </c>
       <c r="G6" t="s">
-        <v>49</v>
+        <v>17</v>
       </c>
       <c r="H6" t="s">
-        <v>49</v>
+        <v>17</v>
       </c>
       <c r="I6" t="s">
-        <v>49</v>
+        <v>17</v>
       </c>
       <c r="J6" t="s">
-        <v>49</v>
+        <v>17</v>
       </c>
       <c r="K6" t="s">
-        <v>49</v>
+        <v>17</v>
       </c>
       <c r="L6" t="s">
-        <v>49</v>
+        <v>17</v>
       </c>
       <c r="M6" t="s">
-        <v>49</v>
+        <v>17</v>
       </c>
       <c r="N6" t="s">
-        <v>49</v>
+        <v>17</v>
       </c>
       <c r="O6" t="s">
-        <v>49</v>
+        <v>17</v>
       </c>
       <c r="P6" t="s">
-        <v>49</v>
+        <v>17</v>
       </c>
       <c r="Q6" t="s">
-        <v>49</v>
+        <v>17</v>
       </c>
       <c r="R6" t="s">
-        <v>49</v>
+        <v>17</v>
       </c>
       <c r="S6" t="s">
-        <v>49</v>
+        <v>17</v>
       </c>
       <c r="T6" t="s">
-        <v>49</v>
+        <v>17</v>
       </c>
       <c r="U6" t="s">
-        <v>49</v>
+        <v>17</v>
       </c>
       <c r="V6" t="s">
-        <v>49</v>
+        <v>17</v>
       </c>
       <c r="W6" t="s">
-        <v>49</v>
+        <v>17</v>
       </c>
       <c r="X6" t="s">
-        <v>49</v>
+        <v>17</v>
       </c>
       <c r="Y6" t="s">
-        <v>49</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
-        <v>33</v>
+        <v>18</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
       <c r="I7" s="5" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
       <c r="J7" s="5" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
       <c r="K7" s="5" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
       <c r="L7" s="5" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
       <c r="M7" s="5" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
       <c r="N7" s="5" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
       <c r="O7" s="5" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
       <c r="P7" s="5" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
       <c r="Q7" s="5" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
       <c r="R7" s="5" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
       <c r="S7" s="5" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
       <c r="T7" s="5" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
       <c r="U7" s="5" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
       <c r="V7" s="5" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
       <c r="W7" s="5" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
       <c r="X7" s="5" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
       <c r="Y7" s="5" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A8" s="2" t="s">
-        <v>29</v>
+      <c r="A8" t="s">
+        <v>20</v>
       </c>
       <c r="B8" s="4">
         <v>2000</v>
@@ -1206,178 +1193,682 @@
     </row>
     <row r="9" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>6</v>
+        <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A10" s="2" t="s">
-        <v>7</v>
-      </c>
+      <c r="A10" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10"/>
+      <c r="C10"/>
+      <c r="D10"/>
+      <c r="E10"/>
+      <c r="F10"/>
+      <c r="G10"/>
+      <c r="H10"/>
+      <c r="I10"/>
+      <c r="J10"/>
+      <c r="K10"/>
+      <c r="L10"/>
+      <c r="M10"/>
+      <c r="N10"/>
+      <c r="O10"/>
+      <c r="P10"/>
+      <c r="Q10"/>
+      <c r="R10"/>
+      <c r="S10"/>
+      <c r="T10"/>
+      <c r="U10"/>
+      <c r="V10"/>
+      <c r="W10"/>
+      <c r="X10"/>
+      <c r="Y10"/>
     </row>
     <row r="11" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A11" s="2" t="s">
-        <v>8</v>
-      </c>
+      <c r="A11" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11"/>
+      <c r="C11"/>
+      <c r="D11"/>
+      <c r="E11"/>
+      <c r="F11"/>
+      <c r="G11"/>
+      <c r="H11"/>
+      <c r="I11"/>
+      <c r="J11"/>
+      <c r="K11"/>
+      <c r="L11"/>
+      <c r="M11"/>
+      <c r="N11"/>
+      <c r="O11"/>
+      <c r="P11"/>
+      <c r="Q11"/>
+      <c r="R11"/>
+      <c r="S11"/>
+      <c r="T11"/>
+      <c r="U11"/>
+      <c r="V11"/>
+      <c r="W11"/>
+      <c r="X11"/>
+      <c r="Y11"/>
     </row>
     <row r="12" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A12" s="2" t="s">
-        <v>9</v>
-      </c>
+      <c r="A12" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12"/>
+      <c r="C12"/>
+      <c r="D12"/>
+      <c r="E12"/>
+      <c r="F12"/>
+      <c r="G12"/>
+      <c r="H12"/>
+      <c r="I12"/>
+      <c r="J12"/>
+      <c r="K12"/>
+      <c r="L12"/>
+      <c r="M12"/>
+      <c r="N12"/>
+      <c r="O12"/>
+      <c r="P12"/>
+      <c r="Q12"/>
+      <c r="R12"/>
+      <c r="S12"/>
+      <c r="T12"/>
+      <c r="U12"/>
+      <c r="V12"/>
+      <c r="W12"/>
+      <c r="X12"/>
+      <c r="Y12"/>
     </row>
     <row r="13" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A13" s="2" t="s">
-        <v>10</v>
-      </c>
+      <c r="A13" t="s">
+        <v>25</v>
+      </c>
+      <c r="B13"/>
+      <c r="C13"/>
+      <c r="D13"/>
+      <c r="E13"/>
+      <c r="F13"/>
+      <c r="G13"/>
+      <c r="H13"/>
+      <c r="I13"/>
+      <c r="J13"/>
+      <c r="K13"/>
+      <c r="L13"/>
+      <c r="M13"/>
+      <c r="N13"/>
+      <c r="O13"/>
+      <c r="P13"/>
+      <c r="Q13"/>
+      <c r="R13"/>
+      <c r="S13"/>
+      <c r="T13"/>
+      <c r="U13"/>
+      <c r="V13"/>
+      <c r="W13"/>
+      <c r="X13"/>
+      <c r="Y13"/>
     </row>
     <row r="14" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A14" s="2" t="s">
-        <v>11</v>
-      </c>
+      <c r="A14" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14"/>
+      <c r="C14"/>
+      <c r="D14"/>
+      <c r="E14"/>
+      <c r="F14"/>
+      <c r="G14"/>
+      <c r="H14"/>
+      <c r="I14"/>
+      <c r="J14"/>
+      <c r="K14"/>
+      <c r="L14"/>
+      <c r="M14"/>
+      <c r="N14"/>
+      <c r="O14"/>
+      <c r="P14"/>
+      <c r="Q14"/>
+      <c r="R14"/>
+      <c r="S14"/>
+      <c r="T14"/>
+      <c r="U14"/>
+      <c r="V14"/>
+      <c r="W14"/>
+      <c r="X14"/>
+      <c r="Y14"/>
     </row>
     <row r="15" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A15" s="2" t="s">
-        <v>12</v>
-      </c>
+      <c r="A15" t="s">
+        <v>27</v>
+      </c>
+      <c r="B15"/>
+      <c r="C15"/>
+      <c r="D15"/>
+      <c r="E15"/>
+      <c r="F15"/>
+      <c r="G15"/>
+      <c r="H15"/>
+      <c r="I15"/>
+      <c r="J15"/>
+      <c r="K15"/>
+      <c r="L15"/>
+      <c r="M15"/>
+      <c r="N15"/>
+      <c r="O15"/>
+      <c r="P15"/>
+      <c r="Q15"/>
+      <c r="R15"/>
+      <c r="S15"/>
+      <c r="T15"/>
+      <c r="U15"/>
+      <c r="V15"/>
+      <c r="W15"/>
+      <c r="X15"/>
+      <c r="Y15"/>
     </row>
     <row r="16" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A16" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A17" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A18" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A19" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A20" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A21" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A22" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A23" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A24" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A25" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A26" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A27" s="2" t="s">
+      <c r="A16" t="s">
+        <v>28</v>
+      </c>
+      <c r="B16"/>
+      <c r="C16"/>
+      <c r="D16"/>
+      <c r="E16"/>
+      <c r="F16"/>
+      <c r="G16"/>
+      <c r="H16"/>
+      <c r="I16"/>
+      <c r="J16"/>
+      <c r="K16"/>
+      <c r="L16"/>
+      <c r="M16"/>
+      <c r="N16"/>
+      <c r="O16"/>
+      <c r="P16"/>
+      <c r="Q16"/>
+      <c r="R16"/>
+      <c r="S16"/>
+      <c r="T16"/>
+      <c r="U16"/>
+      <c r="V16"/>
+      <c r="W16"/>
+      <c r="X16"/>
+      <c r="Y16"/>
+    </row>
+    <row r="17" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>29</v>
+      </c>
+      <c r="B17"/>
+      <c r="C17"/>
+      <c r="D17"/>
+      <c r="E17"/>
+      <c r="F17"/>
+      <c r="G17"/>
+      <c r="H17"/>
+      <c r="I17"/>
+      <c r="J17"/>
+      <c r="K17"/>
+      <c r="L17"/>
+      <c r="M17"/>
+      <c r="N17"/>
+      <c r="O17"/>
+      <c r="P17"/>
+      <c r="Q17"/>
+      <c r="R17"/>
+      <c r="S17"/>
+      <c r="T17"/>
+      <c r="U17"/>
+      <c r="V17"/>
+      <c r="W17"/>
+      <c r="X17"/>
+      <c r="Y17"/>
+    </row>
+    <row r="18" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>30</v>
+      </c>
+      <c r="B18"/>
+      <c r="C18"/>
+      <c r="D18"/>
+      <c r="E18"/>
+      <c r="F18"/>
+      <c r="G18"/>
+      <c r="H18"/>
+      <c r="I18"/>
+      <c r="J18"/>
+      <c r="K18"/>
+      <c r="L18"/>
+      <c r="M18"/>
+      <c r="N18"/>
+      <c r="O18"/>
+      <c r="P18"/>
+      <c r="Q18"/>
+      <c r="R18"/>
+      <c r="S18"/>
+      <c r="T18"/>
+      <c r="U18"/>
+      <c r="V18"/>
+      <c r="W18"/>
+      <c r="X18"/>
+      <c r="Y18"/>
+    </row>
+    <row r="19" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="20" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="21" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="22" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="23" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="24" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="25" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="26" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="27" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="28" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="29" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A28" s="2" t="s">
+    <row r="30" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A29" s="2" t="s">
+    <row r="31" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A30" s="2" t="s">
+      <c r="B31"/>
+      <c r="C31"/>
+      <c r="D31"/>
+      <c r="E31"/>
+      <c r="F31"/>
+      <c r="G31"/>
+      <c r="H31"/>
+      <c r="I31"/>
+      <c r="J31"/>
+      <c r="K31"/>
+      <c r="L31"/>
+      <c r="M31"/>
+      <c r="N31"/>
+      <c r="O31"/>
+      <c r="P31"/>
+      <c r="Q31"/>
+      <c r="R31"/>
+      <c r="S31"/>
+      <c r="T31"/>
+      <c r="U31"/>
+      <c r="V31"/>
+      <c r="W31"/>
+      <c r="X31"/>
+      <c r="Y31"/>
+    </row>
+    <row r="32" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A31" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A32" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A33" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A34" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A35" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B32"/>
+      <c r="C32"/>
+      <c r="D32"/>
+      <c r="E32"/>
+      <c r="F32"/>
+      <c r="G32"/>
+      <c r="H32"/>
+      <c r="I32"/>
+      <c r="J32"/>
+      <c r="K32"/>
+      <c r="L32"/>
+      <c r="M32"/>
+      <c r="N32"/>
+      <c r="O32"/>
+      <c r="P32"/>
+      <c r="Q32"/>
+      <c r="R32"/>
+      <c r="S32"/>
+      <c r="T32"/>
+      <c r="U32"/>
+      <c r="V32"/>
+      <c r="W32"/>
+      <c r="X32"/>
+      <c r="Y32"/>
+    </row>
+    <row r="33" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>45</v>
+      </c>
+      <c r="B33"/>
+      <c r="C33"/>
+      <c r="D33"/>
+      <c r="E33"/>
+      <c r="F33"/>
+      <c r="G33"/>
+      <c r="H33"/>
+      <c r="I33"/>
+      <c r="J33"/>
+      <c r="K33"/>
+      <c r="L33"/>
+      <c r="M33"/>
+      <c r="N33"/>
+      <c r="O33"/>
+      <c r="P33"/>
+      <c r="Q33"/>
+      <c r="R33"/>
+      <c r="S33"/>
+      <c r="T33"/>
+      <c r="U33"/>
+      <c r="V33"/>
+      <c r="W33"/>
+      <c r="X33"/>
+      <c r="Y33"/>
+    </row>
+    <row r="34" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>46</v>
+      </c>
+      <c r="B34"/>
+      <c r="C34"/>
+      <c r="D34"/>
+      <c r="E34"/>
+      <c r="F34"/>
+      <c r="G34"/>
+      <c r="H34"/>
+      <c r="I34"/>
+      <c r="J34"/>
+      <c r="K34"/>
+      <c r="L34"/>
+      <c r="M34"/>
+      <c r="N34"/>
+      <c r="O34"/>
+      <c r="P34"/>
+      <c r="Q34"/>
+      <c r="R34"/>
+      <c r="S34"/>
+      <c r="T34"/>
+      <c r="U34"/>
+      <c r="V34"/>
+      <c r="W34"/>
+      <c r="X34"/>
+      <c r="Y34"/>
+    </row>
+    <row r="35" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>47</v>
+      </c>
+      <c r="B35"/>
+      <c r="C35"/>
+      <c r="D35"/>
+      <c r="E35"/>
+      <c r="F35"/>
+      <c r="G35"/>
+      <c r="H35"/>
+      <c r="I35"/>
+      <c r="J35"/>
+      <c r="K35"/>
+      <c r="L35"/>
+      <c r="M35"/>
+      <c r="N35"/>
+      <c r="O35"/>
+      <c r="P35"/>
+      <c r="Q35"/>
+      <c r="R35"/>
+      <c r="S35"/>
+      <c r="T35"/>
+      <c r="U35"/>
+      <c r="V35"/>
+      <c r="W35"/>
+      <c r="X35"/>
+      <c r="Y35"/>
+    </row>
+    <row r="36" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A37" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A38" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A39" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A40" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A41" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A42" s="2" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A43" s="2" t="s">
         <v>48</v>
       </c>
+    </row>
+    <row r="37" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>49</v>
+      </c>
+      <c r="B37"/>
+      <c r="C37"/>
+      <c r="D37"/>
+      <c r="E37"/>
+      <c r="F37"/>
+      <c r="G37"/>
+      <c r="H37"/>
+      <c r="I37"/>
+      <c r="J37"/>
+      <c r="K37"/>
+      <c r="L37"/>
+      <c r="M37"/>
+      <c r="N37"/>
+      <c r="O37"/>
+      <c r="P37"/>
+      <c r="Q37"/>
+      <c r="R37"/>
+      <c r="S37"/>
+      <c r="T37"/>
+      <c r="U37"/>
+      <c r="V37"/>
+      <c r="W37"/>
+      <c r="X37"/>
+      <c r="Y37"/>
+    </row>
+    <row r="38" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>50</v>
+      </c>
+      <c r="B38"/>
+      <c r="C38"/>
+      <c r="D38"/>
+      <c r="E38"/>
+      <c r="F38"/>
+      <c r="G38"/>
+      <c r="H38"/>
+      <c r="I38"/>
+      <c r="J38"/>
+      <c r="K38"/>
+      <c r="L38"/>
+      <c r="M38"/>
+      <c r="N38"/>
+      <c r="O38"/>
+      <c r="P38"/>
+      <c r="Q38"/>
+      <c r="R38"/>
+      <c r="S38"/>
+      <c r="T38"/>
+      <c r="U38"/>
+      <c r="V38"/>
+      <c r="W38"/>
+      <c r="X38"/>
+      <c r="Y38"/>
+    </row>
+    <row r="39" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>51</v>
+      </c>
+      <c r="B39"/>
+      <c r="C39"/>
+      <c r="D39"/>
+      <c r="E39"/>
+      <c r="F39"/>
+      <c r="G39"/>
+      <c r="H39"/>
+      <c r="I39"/>
+      <c r="J39"/>
+      <c r="K39"/>
+      <c r="L39"/>
+      <c r="M39"/>
+      <c r="N39"/>
+      <c r="O39"/>
+      <c r="P39"/>
+      <c r="Q39"/>
+      <c r="R39"/>
+      <c r="S39"/>
+      <c r="T39"/>
+      <c r="U39"/>
+      <c r="V39"/>
+      <c r="W39"/>
+      <c r="X39"/>
+      <c r="Y39"/>
+    </row>
+    <row r="40" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>52</v>
+      </c>
+      <c r="B40"/>
+      <c r="C40"/>
+      <c r="D40"/>
+      <c r="E40"/>
+      <c r="F40"/>
+      <c r="G40"/>
+      <c r="H40"/>
+      <c r="I40"/>
+      <c r="J40"/>
+      <c r="K40"/>
+      <c r="L40"/>
+      <c r="M40"/>
+      <c r="N40"/>
+      <c r="O40"/>
+      <c r="P40"/>
+      <c r="Q40"/>
+      <c r="R40"/>
+      <c r="S40"/>
+      <c r="T40"/>
+      <c r="U40"/>
+      <c r="V40"/>
+      <c r="W40"/>
+      <c r="X40"/>
+      <c r="Y40"/>
+    </row>
+    <row r="41" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>53</v>
+      </c>
+      <c r="B41"/>
+      <c r="C41"/>
+      <c r="D41"/>
+      <c r="E41"/>
+      <c r="F41"/>
+      <c r="G41"/>
+      <c r="H41"/>
+      <c r="I41"/>
+      <c r="J41"/>
+      <c r="K41"/>
+      <c r="L41"/>
+      <c r="M41"/>
+      <c r="N41"/>
+      <c r="O41"/>
+      <c r="P41"/>
+      <c r="Q41"/>
+      <c r="R41"/>
+      <c r="S41"/>
+      <c r="T41"/>
+      <c r="U41"/>
+      <c r="V41"/>
+      <c r="W41"/>
+      <c r="X41"/>
+      <c r="Y41"/>
+    </row>
+    <row r="42" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>54</v>
+      </c>
+      <c r="B42"/>
+      <c r="C42"/>
+      <c r="D42"/>
+      <c r="E42"/>
+      <c r="F42"/>
+      <c r="G42"/>
+      <c r="H42"/>
+      <c r="I42"/>
+      <c r="J42"/>
+      <c r="K42"/>
+      <c r="L42"/>
+      <c r="M42"/>
+      <c r="N42"/>
+      <c r="O42"/>
+      <c r="P42"/>
+      <c r="Q42"/>
+      <c r="R42"/>
+      <c r="S42"/>
+      <c r="T42"/>
+      <c r="U42"/>
+      <c r="V42"/>
+      <c r="W42"/>
+      <c r="X42"/>
+      <c r="Y42"/>
+    </row>
+    <row r="43" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>55</v>
+      </c>
+      <c r="B43"/>
+      <c r="C43"/>
+      <c r="D43"/>
+      <c r="E43"/>
+      <c r="F43"/>
+      <c r="G43"/>
+      <c r="H43"/>
+      <c r="I43"/>
+      <c r="J43"/>
+      <c r="K43"/>
+      <c r="L43"/>
+      <c r="M43"/>
+      <c r="N43"/>
+      <c r="O43"/>
+      <c r="P43"/>
+      <c r="Q43"/>
+      <c r="R43"/>
+      <c r="S43"/>
+      <c r="T43"/>
+      <c r="U43"/>
+      <c r="V43"/>
+      <c r="W43"/>
+      <c r="X43"/>
+      <c r="Y43"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>